<commit_message>
24/02/2016, haciendo el cambio de monedas
</commit_message>
<xml_diff>
--- a/assets/archivo-prueba-importacion.xlsx
+++ b/assets/archivo-prueba-importacion.xlsx
@@ -2,16 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -111,7 +116,7 @@
     <t>CAT_MEX</t>
   </si>
   <si>
-    <t>LigaM  MX</t>
+    <t>Liga  MX</t>
   </si>
   <si>
     <t>Primera División de México</t>
@@ -154,6 +159,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -224,7 +230,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,14 +265,13 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,14 +465,13 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,7 +650,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>